<commit_message>
refactor: message error style changed
</commit_message>
<xml_diff>
--- a/data/adicional_column.xlsx
+++ b/data/adicional_column.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>email</t>
   </si>
@@ -43,7 +43,7 @@
     <t>Produto A</t>
   </si>
   <si>
-    <t>ds</t>
+    <t>s</t>
   </si>
   <si>
     <t>categoria1</t>
@@ -70,16 +70,10 @@
     <t>Produto D</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>usuario5@example.com</t>
   </si>
   <si>
     <t>Produto E</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>usuario6@example.com</t>
@@ -685,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>10</v>
@@ -693,7 +687,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>44931</v>
@@ -702,13 +696,13 @@
         <v>499.99</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="7">
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
@@ -716,7 +710,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>44932</v>
@@ -725,13 +719,13 @@
         <v>249</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>15</v>
@@ -739,7 +733,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2">
         <v>44933</v>
@@ -748,13 +742,13 @@
         <v>300</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="7">
         <v>4</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>10</v>
@@ -762,7 +756,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2">
         <v>44934</v>
@@ -771,13 +765,13 @@
         <v>450.5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" s="7">
         <v>2</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
@@ -785,7 +779,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2">
         <v>44935</v>
@@ -794,13 +788,13 @@
         <v>129.95</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" s="7">
         <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>15</v>
@@ -808,7 +802,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2">
         <v>44936</v>
@@ -817,13 +811,13 @@
         <v>89.9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="7">
         <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>10</v>
@@ -831,7 +825,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2">
         <v>44937</v>
@@ -840,13 +834,13 @@
         <v>199.9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>12</v>
@@ -854,7 +848,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2">
         <v>44938</v>
@@ -863,13 +857,13 @@
         <v>149.5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="7">
         <v>4</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>15</v>
@@ -877,7 +871,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2">
         <v>44939</v>
@@ -886,13 +880,13 @@
         <v>229</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" s="7">
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
@@ -900,7 +894,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2">
         <v>44940</v>
@@ -909,13 +903,13 @@
         <v>309.99</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="7">
         <v>2</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>12</v>
@@ -923,7 +917,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2">
         <v>44941</v>
@@ -932,13 +926,13 @@
         <v>399</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>15</v>
@@ -946,7 +940,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2">
         <v>44942</v>
@@ -955,13 +949,13 @@
         <v>129</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E17" s="7">
         <v>5</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>10</v>
@@ -969,7 +963,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2">
         <v>44943</v>
@@ -978,13 +972,13 @@
         <v>159.99</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="7">
         <v>2</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>12</v>
@@ -992,7 +986,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2">
         <v>44944</v>
@@ -1001,13 +995,13 @@
         <v>289.95</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E19" s="7">
         <v>3</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>15</v>
@@ -1015,7 +1009,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="2">
         <v>44945</v>
@@ -1024,13 +1018,13 @@
         <v>349.9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7">
         <v>4</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>10</v>
@@ -1038,7 +1032,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2">
         <v>44946</v>
@@ -1047,13 +1041,13 @@
         <v>399.99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="7">
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>12</v>

</xml_diff>